<commit_message>
Update to use car models
</commit_message>
<xml_diff>
--- a/test_data/models.xlsx
+++ b/test_data/models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\powerBIModelViewer\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0FF5FA-529C-40EF-B670-083BE6B32E5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8688102-70E7-42AF-A7E6-F320E3BCF240}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="840" windowWidth="28800" windowHeight="11990" xr2:uid="{5CB7E3B4-95EB-4C43-8A6D-3D554C135EFF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="70">
   <si>
     <t>Names</t>
   </si>
@@ -41,44 +41,226 @@
     <t>Source</t>
   </si>
   <si>
-    <t>https://cdn.glitch.com/36cb8393-65c6-408d-a538-055ada20431b/Astronaut.glb?1542147958948</t>
-  </si>
-  <si>
-    <t>https://cdn.glitch.com/90a30469-f038-4054-be9c-fd1ec94a810d%2Fkitchentest.glb?1537178470645</t>
-  </si>
-  <si>
-    <t>https://cdn.glitch.com/162a6be2-293d-4554-8610-6011a9f71fef%2FChairExp.glb?1557485499409</t>
-  </si>
-  <si>
-    <t>https://cdn.glitch.com/32f1ec0f-1e16-448a-b891-71f24804e417%2FDuck.glb?v=1561641862851</t>
-  </si>
-  <si>
-    <t>Astronaut.glb</t>
-  </si>
-  <si>
-    <t>kitchentest.glb</t>
-  </si>
-  <si>
-    <t>ChairExp.glb</t>
-  </si>
-  <si>
-    <t>Duck.glb</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>glTF</t>
+    <t>van.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/van.glb</t>
+  </si>
+  <si>
+    <t>Poster</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/ambulance.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/delivery.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/deliveryFlat.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/firetruck.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/garbageTruck.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/hatchbackSports.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/police.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/race.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/raceFuture.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/sedan.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/sedanSports.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/suv.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/suvLuxury.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/taxi.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/tractor.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/tractorPolice.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/tractorShovel.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/truck.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/truckFlat.glb</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/ambulance_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/delivery_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/deliveryFlat_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/firetruck_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/garbageTruck_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/hatchbackSports_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/police_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/race_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/raceFuture_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/sedan_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/sedanSports_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/suv_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/suvLuxury_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/taxi_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/tractor_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/tractorPolice_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/tractorShovel_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/truck_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/truckFlat_SE.png</t>
+  </si>
+  <si>
+    <t>https://kelleyma49.github.io/powerBIModelViewer/example_models/van_SE.png</t>
+  </si>
+  <si>
+    <t>ambulance.glb</t>
+  </si>
+  <si>
+    <t>delivery.glb</t>
+  </si>
+  <si>
+    <t>deliveryFlat.glb</t>
+  </si>
+  <si>
+    <t>firetruck.glb</t>
+  </si>
+  <si>
+    <t>garbageTruck.glb</t>
+  </si>
+  <si>
+    <t>hatchbackSports.glb</t>
+  </si>
+  <si>
+    <t>police.glb</t>
+  </si>
+  <si>
+    <t>race.glb</t>
+  </si>
+  <si>
+    <t>raceFuture.glb</t>
+  </si>
+  <si>
+    <t>sedan.glb</t>
+  </si>
+  <si>
+    <t>sedanSports.glb</t>
+  </si>
+  <si>
+    <t>suv.glb</t>
+  </si>
+  <si>
+    <t>suvLuxury.glb</t>
+  </si>
+  <si>
+    <t>taxi.glb</t>
+  </si>
+  <si>
+    <t>tractor.glb</t>
+  </si>
+  <si>
+    <t>tractorPolice.glb</t>
+  </si>
+  <si>
+    <t>tractorShovel.glb</t>
+  </si>
+  <si>
+    <t>truck.glb</t>
+  </si>
+  <si>
+    <t>truckFlat.glb</t>
+  </si>
+  <si>
+    <t>Primary Color</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>White</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,13 +283,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -420,19 +605,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C06A676-9252-4B51-A6F7-E8C23304DAFB}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="84.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,55 +626,297 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B21" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C9" r:id="rId1" xr:uid="{0962095F-C4DA-4E61-B2A4-A64F181FFA78}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>